<commit_message>
Final Regressions and tables
</commit_message>
<xml_diff>
--- a/Results_Tables/Uganda_Final_Tables.xlsx
+++ b/Results_Tables/Uganda_Final_Tables.xlsx
@@ -5,19 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CGIAR\Uganda\Report &amp; Results Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CGIAR\Uganda\Results_Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Neg_rainfall_stunt_battles" sheetId="17" r:id="rId1"/>
     <sheet name="Neg_rainfall_stunt_riots" sheetId="18" r:id="rId2"/>
     <sheet name="Neg_rainfall_stunt_VAC" sheetId="19" r:id="rId3"/>
-    <sheet name="Neg_rainfall_maize_battles" sheetId="15" r:id="rId4"/>
-    <sheet name="Neg_rainfall_maize_riots" sheetId="16" r:id="rId5"/>
-    <sheet name="Foglio1" sheetId="1" r:id="rId6"/>
+    <sheet name="Neg_rainfall_stunt_Protests" sheetId="20" r:id="rId4"/>
+    <sheet name="Neg_rainfall_maize_battles" sheetId="15" r:id="rId5"/>
+    <sheet name="Neg_rainfall_maize_riots" sheetId="16" r:id="rId6"/>
+    <sheet name="Foglio1" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1734" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2087" uniqueCount="518">
   <si>
     <t>MAIN SPECIFICATION</t>
   </si>
@@ -1511,6 +1512,87 @@
   </si>
   <si>
     <t>(0.322)</t>
+  </si>
+  <si>
+    <t>Future Violence - Protests (log)</t>
+  </si>
+  <si>
+    <t>Positive_temperature_stunt_Protests</t>
+  </si>
+  <si>
+    <t>(0.023)</t>
+  </si>
+  <si>
+    <t>0.123**</t>
+  </si>
+  <si>
+    <t>(0.017)</t>
+  </si>
+  <si>
+    <t>-0.094***</t>
+  </si>
+  <si>
+    <t>-0.103***</t>
+  </si>
+  <si>
+    <t>-0.100**</t>
+  </si>
+  <si>
+    <t>-0.030</t>
+  </si>
+  <si>
+    <t>(0.150)</t>
+  </si>
+  <si>
+    <t>0.070***</t>
+  </si>
+  <si>
+    <t>-0.092***</t>
+  </si>
+  <si>
+    <t>0.071**</t>
+  </si>
+  <si>
+    <t>0.071</t>
+  </si>
+  <si>
+    <t>-0.090***</t>
+  </si>
+  <si>
+    <t>0.047</t>
+  </si>
+  <si>
+    <t>0.083*</t>
+  </si>
+  <si>
+    <t>-0.096***</t>
+  </si>
+  <si>
+    <t>-0.019</t>
+  </si>
+  <si>
+    <t>0.059</t>
+  </si>
+  <si>
+    <t>-0.097***</t>
+  </si>
+  <si>
+    <t>-0.098***</t>
+  </si>
+  <si>
+    <t>-0.000</t>
+  </si>
+  <si>
+    <t>0.080*</t>
+  </si>
+  <si>
+    <t>-0.095***</t>
+  </si>
+  <si>
+    <t>0.006</t>
+  </si>
+  <si>
+    <t>(0.122)</t>
   </si>
 </sst>
 </file>
@@ -1662,7 +1744,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1717,11 +1799,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1842,20 +1933,8 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1883,6 +1962,21 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2224,22 +2318,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="D3" s="60">
+      <c r="D3" s="56">
         <v>1</v>
       </c>
-      <c r="E3" s="60">
+      <c r="E3" s="56">
         <v>2</v>
       </c>
       <c r="F3" s="28">
@@ -2248,16 +2342,16 @@
       <c r="G3" s="28">
         <v>4</v>
       </c>
-      <c r="H3" s="60">
+      <c r="H3" s="56">
         <v>5</v>
       </c>
-      <c r="I3" s="60">
+      <c r="I3" s="56">
         <v>6</v>
       </c>
-      <c r="J3" s="60">
+      <c r="J3" s="56">
         <v>7</v>
       </c>
-      <c r="K3" s="60">
+      <c r="K3" s="56">
         <v>8</v>
       </c>
     </row>
@@ -2294,7 +2388,7 @@
       <c r="C5" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="58" t="s">
         <v>265</v>
       </c>
       <c r="E5" s="44" t="s">
@@ -2305,7 +2399,7 @@
       <c r="C6" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="62" t="s">
+      <c r="D6" s="58" t="s">
         <v>267</v>
       </c>
       <c r="E6" s="44" t="s">
@@ -2321,7 +2415,7 @@
       <c r="F7" s="44" t="s">
         <v>282</v>
       </c>
-      <c r="G7" s="62" t="s">
+      <c r="G7" s="58" t="s">
         <v>283</v>
       </c>
     </row>
@@ -2334,7 +2428,7 @@
       <c r="F8" s="44" t="s">
         <v>284</v>
       </c>
-      <c r="G8" s="62" t="s">
+      <c r="G8" s="58" t="s">
         <v>285</v>
       </c>
     </row>
@@ -2344,8 +2438,8 @@
       </c>
       <c r="D9" s="46"/>
       <c r="E9" s="46"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
       <c r="H9" s="44" t="s">
         <v>308</v>
       </c>
@@ -2359,8 +2453,8 @@
       </c>
       <c r="D10" s="46"/>
       <c r="E10" s="46"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
       <c r="H10" s="44" t="s">
         <v>292</v>
       </c>
@@ -2376,7 +2470,7 @@
       <c r="E11" s="46"/>
       <c r="H11" s="44"/>
       <c r="I11" s="44"/>
-      <c r="J11" s="62" t="s">
+      <c r="J11" s="58" t="s">
         <v>320</v>
       </c>
       <c r="K11" s="44" t="s">
@@ -2389,9 +2483,9 @@
       </c>
       <c r="D12" s="46"/>
       <c r="E12" s="46"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="62" t="s">
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="58" t="s">
         <v>322</v>
       </c>
       <c r="K12" s="44" t="s">
@@ -2403,16 +2497,16 @@
         <v>110</v>
       </c>
       <c r="D13" s="46"/>
-      <c r="E13" s="62" t="s">
+      <c r="E13" s="58" t="s">
         <v>263</v>
       </c>
       <c r="G13" s="44">
         <v>0.113</v>
       </c>
-      <c r="I13" s="62" t="s">
+      <c r="I13" s="58" t="s">
         <v>307</v>
       </c>
-      <c r="K13" s="62" t="s">
+      <c r="K13" s="58" t="s">
         <v>319</v>
       </c>
     </row>
@@ -2421,16 +2515,16 @@
         <v>4</v>
       </c>
       <c r="D14" s="46"/>
-      <c r="E14" s="62" t="s">
+      <c r="E14" s="58" t="s">
         <v>264</v>
       </c>
       <c r="G14" s="44" t="s">
         <v>286</v>
       </c>
-      <c r="I14" s="62" t="s">
+      <c r="I14" s="58" t="s">
         <v>264</v>
       </c>
-      <c r="K14" s="62" t="s">
+      <c r="K14" s="58" t="s">
         <v>264</v>
       </c>
     </row>
@@ -2661,7 +2755,7 @@
       </c>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C23" s="51" t="s">
+      <c r="C23" s="48" t="s">
         <v>101</v>
       </c>
       <c r="D23" s="44" t="s">
@@ -2729,28 +2823,28 @@
       <c r="C26" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="54" t="s">
+      <c r="D26" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="E26" s="54" t="s">
+      <c r="E26" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="F26" s="54" t="s">
+      <c r="F26" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="G26" s="54" t="s">
+      <c r="G26" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="H26" s="54" t="s">
+      <c r="H26" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="I26" s="54" t="s">
+      <c r="I26" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="J26" s="54" t="s">
+      <c r="J26" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="K26" s="54" t="s">
+      <c r="K26" s="50" t="s">
         <v>281</v>
       </c>
     </row>
@@ -2813,7 +2907,7 @@
       </c>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C29" s="61" t="s">
+      <c r="C29" s="57" t="s">
         <v>86</v>
       </c>
       <c r="D29" s="31" t="s">
@@ -2912,7 +3006,7 @@
       <c r="F32" s="41">
         <v>0.1586331</v>
       </c>
-      <c r="G32" s="55">
+      <c r="G32" s="51">
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="H32" s="41">
@@ -2970,7 +3064,7 @@
       <c r="F34" s="41">
         <v>0.16094820000000001</v>
       </c>
-      <c r="G34" s="55">
+      <c r="G34" s="51">
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="H34" s="47">
@@ -3020,22 +3114,22 @@
       </c>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="D44" s="52" t="s">
+      <c r="D44" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="E44" s="52"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="52"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="52"/>
-      <c r="K44" s="52"/>
+      <c r="E44" s="59"/>
+      <c r="F44" s="59"/>
+      <c r="G44" s="59"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
+      <c r="K44" s="59"/>
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="D45" s="60">
+      <c r="D45" s="56">
         <v>1</v>
       </c>
-      <c r="E45" s="60">
+      <c r="E45" s="56">
         <v>2</v>
       </c>
       <c r="F45" s="28">
@@ -3044,16 +3138,16 @@
       <c r="G45" s="28">
         <v>4</v>
       </c>
-      <c r="H45" s="60">
+      <c r="H45" s="56">
         <v>5</v>
       </c>
-      <c r="I45" s="60">
+      <c r="I45" s="56">
         <v>6</v>
       </c>
-      <c r="J45" s="60">
+      <c r="J45" s="56">
         <v>7</v>
       </c>
-      <c r="K45" s="60">
+      <c r="K45" s="56">
         <v>8</v>
       </c>
     </row>
@@ -3140,8 +3234,8 @@
       </c>
       <c r="D51" s="46"/>
       <c r="E51" s="46"/>
-      <c r="F51" s="53"/>
-      <c r="G51" s="53"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="49"/>
       <c r="H51" s="44" t="s">
         <v>33</v>
       </c>
@@ -3155,8 +3249,8 @@
       </c>
       <c r="D52" s="46"/>
       <c r="E52" s="46"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="53"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="49"/>
       <c r="H52" s="44" t="s">
         <v>363</v>
       </c>
@@ -3185,8 +3279,8 @@
       </c>
       <c r="D54" s="46"/>
       <c r="E54" s="46"/>
-      <c r="H54" s="53"/>
-      <c r="I54" s="53"/>
+      <c r="H54" s="49"/>
+      <c r="I54" s="49"/>
       <c r="J54" s="44" t="s">
         <v>245</v>
       </c>
@@ -3199,16 +3293,16 @@
         <v>110</v>
       </c>
       <c r="D55" s="46"/>
-      <c r="E55" s="62" t="s">
+      <c r="E55" s="58" t="s">
         <v>343</v>
       </c>
-      <c r="G55" s="62" t="s">
+      <c r="G55" s="58" t="s">
         <v>352</v>
       </c>
-      <c r="I55" s="62" t="s">
+      <c r="I55" s="58" t="s">
         <v>361</v>
       </c>
-      <c r="K55" s="62" t="s">
+      <c r="K55" s="58" t="s">
         <v>335</v>
       </c>
     </row>
@@ -3217,16 +3311,16 @@
         <v>4</v>
       </c>
       <c r="D56" s="46"/>
-      <c r="E56" s="62" t="s">
+      <c r="E56" s="58" t="s">
         <v>264</v>
       </c>
-      <c r="G56" s="62" t="s">
+      <c r="G56" s="58" t="s">
         <v>264</v>
       </c>
-      <c r="I56" s="62" t="s">
+      <c r="I56" s="58" t="s">
         <v>264</v>
       </c>
-      <c r="K56" s="62" t="s">
+      <c r="K56" s="58" t="s">
         <v>264</v>
       </c>
     </row>
@@ -3457,7 +3551,7 @@
       </c>
     </row>
     <row r="65" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C65" s="51" t="s">
+      <c r="C65" s="48" t="s">
         <v>101</v>
       </c>
       <c r="D65" s="44" t="s">
@@ -3525,28 +3619,28 @@
       <c r="C68" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D68" s="54" t="s">
+      <c r="D68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="E68" s="54" t="s">
+      <c r="E68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="F68" s="54" t="s">
+      <c r="F68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="G68" s="54" t="s">
+      <c r="G68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="H68" s="54" t="s">
+      <c r="H68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="I68" s="54" t="s">
+      <c r="I68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="J68" s="54" t="s">
+      <c r="J68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="K68" s="54" t="s">
+      <c r="K68" s="50" t="s">
         <v>281</v>
       </c>
     </row>
@@ -3609,7 +3703,7 @@
       </c>
     </row>
     <row r="71" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C71" s="61" t="s">
+      <c r="C71" s="57" t="s">
         <v>86</v>
       </c>
       <c r="D71" s="31" t="s">
@@ -3821,7 +3915,7 @@
   <dimension ref="C2:K79"/>
   <sheetViews>
     <sheetView zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3840,22 +3934,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="D3" s="60">
+      <c r="D3" s="56">
         <v>1</v>
       </c>
-      <c r="E3" s="60">
+      <c r="E3" s="56">
         <v>2</v>
       </c>
       <c r="F3" s="28">
@@ -3864,16 +3958,16 @@
       <c r="G3" s="28">
         <v>4</v>
       </c>
-      <c r="H3" s="60">
+      <c r="H3" s="56">
         <v>5</v>
       </c>
-      <c r="I3" s="60">
+      <c r="I3" s="56">
         <v>6</v>
       </c>
-      <c r="J3" s="60">
+      <c r="J3" s="56">
         <v>7</v>
       </c>
-      <c r="K3" s="60">
+      <c r="K3" s="56">
         <v>8</v>
       </c>
     </row>
@@ -3910,7 +4004,7 @@
       <c r="C5" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="58" t="s">
         <v>371</v>
       </c>
       <c r="E5" s="44" t="s">
@@ -3921,7 +4015,7 @@
       <c r="C6" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="62" t="s">
+      <c r="D6" s="58" t="s">
         <v>267</v>
       </c>
       <c r="E6" s="44" t="s">
@@ -3960,8 +4054,8 @@
       </c>
       <c r="D9" s="46"/>
       <c r="E9" s="46"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
       <c r="H9" s="44" t="s">
         <v>229</v>
       </c>
@@ -3975,8 +4069,8 @@
       </c>
       <c r="D10" s="46"/>
       <c r="E10" s="46"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
       <c r="H10" s="44" t="s">
         <v>292</v>
       </c>
@@ -3992,10 +4086,10 @@
       <c r="E11" s="46"/>
       <c r="H11" s="44"/>
       <c r="I11" s="44"/>
-      <c r="J11" s="62" t="s">
+      <c r="J11" s="58" t="s">
         <v>399</v>
       </c>
-      <c r="K11" s="62" t="s">
+      <c r="K11" s="58" t="s">
         <v>400</v>
       </c>
     </row>
@@ -4005,12 +4099,12 @@
       </c>
       <c r="D12" s="46"/>
       <c r="E12" s="46"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="62" t="s">
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="58" t="s">
         <v>322</v>
       </c>
-      <c r="K12" s="62" t="s">
+      <c r="K12" s="58" t="s">
         <v>401</v>
       </c>
     </row>
@@ -4277,7 +4371,7 @@
       </c>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C23" s="51" t="s">
+      <c r="C23" s="48" t="s">
         <v>101</v>
       </c>
       <c r="D23" s="44" t="s">
@@ -4337,28 +4431,28 @@
       <c r="C26" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="54" t="s">
+      <c r="D26" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="E26" s="54" t="s">
+      <c r="E26" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="F26" s="54" t="s">
+      <c r="F26" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="G26" s="54" t="s">
+      <c r="G26" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="H26" s="54" t="s">
+      <c r="H26" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="I26" s="54" t="s">
+      <c r="I26" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="J26" s="54" t="s">
+      <c r="J26" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="K26" s="54" t="s">
+      <c r="K26" s="50" t="s">
         <v>281</v>
       </c>
     </row>
@@ -4421,7 +4515,7 @@
       </c>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C29" s="61" t="s">
+      <c r="C29" s="57" t="s">
         <v>86</v>
       </c>
       <c r="D29" s="31" t="s">
@@ -4532,7 +4626,7 @@
       <c r="J32" s="45">
         <v>8.9615399999999998E-2</v>
       </c>
-      <c r="K32" s="55">
+      <c r="K32" s="51">
         <v>6.2E-2</v>
       </c>
     </row>
@@ -4590,7 +4684,7 @@
       <c r="J34" s="41">
         <v>8.8121900000000003E-2</v>
       </c>
-      <c r="K34" s="55">
+      <c r="K34" s="51">
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
@@ -4628,22 +4722,22 @@
       </c>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="D44" s="52" t="s">
+      <c r="D44" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="E44" s="52"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="52"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="52"/>
-      <c r="K44" s="52"/>
+      <c r="E44" s="59"/>
+      <c r="F44" s="59"/>
+      <c r="G44" s="59"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
+      <c r="K44" s="59"/>
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="D45" s="60">
+      <c r="D45" s="56">
         <v>1</v>
       </c>
-      <c r="E45" s="60">
+      <c r="E45" s="56">
         <v>2</v>
       </c>
       <c r="F45" s="28">
@@ -4652,16 +4746,16 @@
       <c r="G45" s="28">
         <v>4</v>
       </c>
-      <c r="H45" s="60">
+      <c r="H45" s="56">
         <v>5</v>
       </c>
-      <c r="I45" s="60">
+      <c r="I45" s="56">
         <v>6</v>
       </c>
-      <c r="J45" s="60">
+      <c r="J45" s="56">
         <v>7</v>
       </c>
-      <c r="K45" s="60">
+      <c r="K45" s="56">
         <v>8</v>
       </c>
     </row>
@@ -4748,8 +4842,8 @@
       </c>
       <c r="D51" s="46"/>
       <c r="E51" s="46"/>
-      <c r="F51" s="53"/>
-      <c r="G51" s="53"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="49"/>
       <c r="H51" s="44" t="s">
         <v>302</v>
       </c>
@@ -4763,8 +4857,8 @@
       </c>
       <c r="D52" s="46"/>
       <c r="E52" s="46"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="53"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="49"/>
       <c r="H52" s="44" t="s">
         <v>363</v>
       </c>
@@ -4793,8 +4887,8 @@
       </c>
       <c r="D54" s="46"/>
       <c r="E54" s="46"/>
-      <c r="H54" s="53"/>
-      <c r="I54" s="53"/>
+      <c r="H54" s="49"/>
+      <c r="I54" s="49"/>
       <c r="J54" s="44" t="s">
         <v>245</v>
       </c>
@@ -5065,7 +5159,7 @@
       </c>
     </row>
     <row r="65" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C65" s="51" t="s">
+      <c r="C65" s="48" t="s">
         <v>101</v>
       </c>
       <c r="D65" s="44" t="s">
@@ -5133,28 +5227,28 @@
       <c r="C68" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D68" s="54" t="s">
+      <c r="D68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="E68" s="54" t="s">
+      <c r="E68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="F68" s="54" t="s">
+      <c r="F68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="G68" s="54" t="s">
+      <c r="G68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="H68" s="54" t="s">
+      <c r="H68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="I68" s="54" t="s">
+      <c r="I68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="J68" s="54" t="s">
+      <c r="J68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="K68" s="54" t="s">
+      <c r="K68" s="50" t="s">
         <v>281</v>
       </c>
     </row>
@@ -5217,7 +5311,7 @@
       </c>
     </row>
     <row r="71" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C71" s="61" t="s">
+      <c r="C71" s="57" t="s">
         <v>86</v>
       </c>
       <c r="D71" s="31" t="s">
@@ -5429,8 +5523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:K79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
-      <selection activeCell="L60" sqref="L60"/>
+    <sheetView topLeftCell="A40" zoomScale="52" zoomScaleNormal="52" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -5449,22 +5543,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="D3" s="60">
+      <c r="D3" s="56">
         <v>1</v>
       </c>
-      <c r="E3" s="60">
+      <c r="E3" s="56">
         <v>2</v>
       </c>
       <c r="F3" s="28">
@@ -5473,16 +5567,16 @@
       <c r="G3" s="28">
         <v>4</v>
       </c>
-      <c r="H3" s="60">
+      <c r="H3" s="56">
         <v>5</v>
       </c>
-      <c r="I3" s="60">
+      <c r="I3" s="56">
         <v>6</v>
       </c>
-      <c r="J3" s="60">
+      <c r="J3" s="56">
         <v>7</v>
       </c>
-      <c r="K3" s="60">
+      <c r="K3" s="56">
         <v>8</v>
       </c>
     </row>
@@ -5519,7 +5613,7 @@
       <c r="C5" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="58" t="s">
         <v>436</v>
       </c>
       <c r="E5" s="44" t="s">
@@ -5530,7 +5624,7 @@
       <c r="C6" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="62" t="s">
+      <c r="D6" s="58" t="s">
         <v>49</v>
       </c>
       <c r="E6" s="44" t="s">
@@ -5569,8 +5663,8 @@
       </c>
       <c r="D9" s="46"/>
       <c r="E9" s="46"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
       <c r="H9" s="44" t="s">
         <v>460</v>
       </c>
@@ -5584,8 +5678,8 @@
       </c>
       <c r="D10" s="46"/>
       <c r="E10" s="46"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
       <c r="H10" s="44" t="s">
         <v>292</v>
       </c>
@@ -5601,7 +5695,7 @@
       <c r="E11" s="46"/>
       <c r="H11" s="44"/>
       <c r="I11" s="44"/>
-      <c r="J11" s="62" t="s">
+      <c r="J11" s="58" t="s">
         <v>320</v>
       </c>
       <c r="K11" s="44" t="s">
@@ -5614,9 +5708,9 @@
       </c>
       <c r="D12" s="46"/>
       <c r="E12" s="46"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="62" t="s">
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="58" t="s">
         <v>322</v>
       </c>
       <c r="K12" s="44" t="s">
@@ -5886,7 +5980,7 @@
       </c>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C23" s="51" t="s">
+      <c r="C23" s="48" t="s">
         <v>101</v>
       </c>
       <c r="D23" s="44" t="s">
@@ -5954,28 +6048,28 @@
       <c r="C26" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="54" t="s">
+      <c r="D26" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="E26" s="54" t="s">
+      <c r="E26" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="F26" s="54" t="s">
+      <c r="F26" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="G26" s="54" t="s">
+      <c r="G26" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="H26" s="54" t="s">
+      <c r="H26" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="I26" s="54" t="s">
+      <c r="I26" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="J26" s="54" t="s">
+      <c r="J26" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="K26" s="54" t="s">
+      <c r="K26" s="50" t="s">
         <v>281</v>
       </c>
     </row>
@@ -6038,7 +6132,7 @@
       </c>
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C29" s="61" t="s">
+      <c r="C29" s="57" t="s">
         <v>86</v>
       </c>
       <c r="D29" s="31" t="s">
@@ -6245,22 +6339,22 @@
       </c>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="D44" s="52" t="s">
+      <c r="D44" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="E44" s="52"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="52"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="52"/>
-      <c r="K44" s="52"/>
+      <c r="E44" s="59"/>
+      <c r="F44" s="59"/>
+      <c r="G44" s="59"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
+      <c r="K44" s="59"/>
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="D45" s="60">
+      <c r="D45" s="56">
         <v>1</v>
       </c>
-      <c r="E45" s="60">
+      <c r="E45" s="56">
         <v>2</v>
       </c>
       <c r="F45" s="28">
@@ -6269,16 +6363,16 @@
       <c r="G45" s="28">
         <v>4</v>
       </c>
-      <c r="H45" s="60">
+      <c r="H45" s="56">
         <v>5</v>
       </c>
-      <c r="I45" s="60">
+      <c r="I45" s="56">
         <v>6</v>
       </c>
-      <c r="J45" s="60">
+      <c r="J45" s="56">
         <v>7</v>
       </c>
-      <c r="K45" s="60">
+      <c r="K45" s="56">
         <v>8</v>
       </c>
     </row>
@@ -6365,8 +6459,8 @@
       </c>
       <c r="D51" s="46"/>
       <c r="E51" s="46"/>
-      <c r="F51" s="53"/>
-      <c r="G51" s="53"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="49"/>
       <c r="H51" s="44" t="s">
         <v>481</v>
       </c>
@@ -6380,8 +6474,8 @@
       </c>
       <c r="D52" s="46"/>
       <c r="E52" s="46"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="53"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="49"/>
       <c r="H52" s="44" t="s">
         <v>363</v>
       </c>
@@ -6410,8 +6504,8 @@
       </c>
       <c r="D54" s="46"/>
       <c r="E54" s="46"/>
-      <c r="H54" s="53"/>
-      <c r="I54" s="53"/>
+      <c r="H54" s="49"/>
+      <c r="I54" s="49"/>
       <c r="J54" s="44" t="s">
         <v>245</v>
       </c>
@@ -6682,7 +6776,7 @@
       </c>
     </row>
     <row r="65" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C65" s="51" t="s">
+      <c r="C65" s="48" t="s">
         <v>101</v>
       </c>
       <c r="D65" s="44" t="s">
@@ -6750,28 +6844,28 @@
       <c r="C68" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D68" s="54" t="s">
+      <c r="D68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="E68" s="54" t="s">
+      <c r="E68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="F68" s="54" t="s">
+      <c r="F68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="G68" s="54" t="s">
+      <c r="G68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="H68" s="54" t="s">
+      <c r="H68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="I68" s="54" t="s">
+      <c r="I68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="J68" s="54" t="s">
+      <c r="J68" s="50" t="s">
         <v>281</v>
       </c>
-      <c r="K68" s="54" t="s">
+      <c r="K68" s="50" t="s">
         <v>281</v>
       </c>
     </row>
@@ -6834,7 +6928,7 @@
       </c>
     </row>
     <row r="71" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C71" s="61" t="s">
+      <c r="C71" s="57" t="s">
         <v>86</v>
       </c>
       <c r="D71" s="31" t="s">
@@ -7042,6 +7136,1562 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:K79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="8.6640625" style="27"/>
+    <col min="3" max="3" width="37.08203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.6640625" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="D2" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+    </row>
+    <row r="3" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="D3" s="56">
+        <v>1</v>
+      </c>
+      <c r="E3" s="56">
+        <v>2</v>
+      </c>
+      <c r="F3" s="28">
+        <v>3</v>
+      </c>
+      <c r="G3" s="28">
+        <v>4</v>
+      </c>
+      <c r="H3" s="56">
+        <v>5</v>
+      </c>
+      <c r="I3" s="56">
+        <v>6</v>
+      </c>
+      <c r="J3" s="56">
+        <v>7</v>
+      </c>
+      <c r="K3" s="56">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>491</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>491</v>
+      </c>
+      <c r="H4" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="I4" s="43" t="s">
+        <v>491</v>
+      </c>
+      <c r="J4" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="K4" s="43" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" ht="16" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="58" t="s">
+        <v>494</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C6" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="44" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C7" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="44" t="s">
+        <v>282</v>
+      </c>
+      <c r="G7" s="44" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="44" t="s">
+        <v>284</v>
+      </c>
+      <c r="G8" s="44" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C9" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="44" t="s">
+        <v>460</v>
+      </c>
+      <c r="I9" s="44" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C10" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="44" t="s">
+        <v>292</v>
+      </c>
+      <c r="I10" s="44" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C11" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="58" t="s">
+        <v>503</v>
+      </c>
+      <c r="K11" s="44" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C12" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="58" t="s">
+        <v>322</v>
+      </c>
+      <c r="K12" s="44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C13" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="46"/>
+      <c r="E13" s="44" t="s">
+        <v>481</v>
+      </c>
+      <c r="G13" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="44" t="s">
+        <v>481</v>
+      </c>
+      <c r="K13" s="44" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C14" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="46"/>
+      <c r="E14" s="44" t="s">
+        <v>493</v>
+      </c>
+      <c r="G14" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="44" t="s">
+        <v>493</v>
+      </c>
+      <c r="K14" s="44" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C15" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>479</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>417</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>287</v>
+      </c>
+      <c r="G15" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="H15" s="44" t="s">
+        <v>501</v>
+      </c>
+      <c r="I15" s="44" t="s">
+        <v>377</v>
+      </c>
+      <c r="J15" s="44" t="s">
+        <v>372</v>
+      </c>
+      <c r="K15" s="44" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C16" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>495</v>
+      </c>
+      <c r="F16" s="44" t="s">
+        <v>245</v>
+      </c>
+      <c r="G16" s="44" t="s">
+        <v>493</v>
+      </c>
+      <c r="H16" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="44" t="s">
+        <v>495</v>
+      </c>
+      <c r="J16" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="K16" s="44" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C17" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="44" t="s">
+        <v>272</v>
+      </c>
+      <c r="E17" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="F17" s="44" t="s">
+        <v>290</v>
+      </c>
+      <c r="G17" s="44" t="s">
+        <v>497</v>
+      </c>
+      <c r="H17" s="44" t="s">
+        <v>272</v>
+      </c>
+      <c r="I17" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="J17" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="K17" s="44" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="D18" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="E18" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="F18" s="44" t="s">
+        <v>292</v>
+      </c>
+      <c r="G18" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="I18" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="J18" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="K18" s="44" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C19" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>443</v>
+      </c>
+      <c r="E19" s="44" t="s">
+        <v>496</v>
+      </c>
+      <c r="F19" s="44" t="s">
+        <v>489</v>
+      </c>
+      <c r="G19" s="44" t="s">
+        <v>498</v>
+      </c>
+      <c r="H19" s="44" t="s">
+        <v>273</v>
+      </c>
+      <c r="I19" s="44" t="s">
+        <v>502</v>
+      </c>
+      <c r="J19" s="44" t="s">
+        <v>504</v>
+      </c>
+      <c r="K19" s="44" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="D20" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="F20" s="44" t="s">
+        <v>465</v>
+      </c>
+      <c r="G20" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="H20" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="J20" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="K20" s="44" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C21" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="44" t="s">
+        <v>288</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>377</v>
+      </c>
+      <c r="F21" s="44" t="s">
+        <v>499</v>
+      </c>
+      <c r="G21" s="44" t="s">
+        <v>427</v>
+      </c>
+      <c r="H21" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="I21" s="44" t="s">
+        <v>247</v>
+      </c>
+      <c r="J21" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="K21" s="44" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C22" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="44" t="s">
+        <v>276</v>
+      </c>
+      <c r="E22" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="44" t="s">
+        <v>300</v>
+      </c>
+      <c r="G22" s="44" t="s">
+        <v>500</v>
+      </c>
+      <c r="H22" s="44" t="s">
+        <v>276</v>
+      </c>
+      <c r="I22" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22" s="44" t="s">
+        <v>276</v>
+      </c>
+      <c r="K22" s="44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C23" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C24" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C25" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C26" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="63" t="s">
+        <v>281</v>
+      </c>
+      <c r="E26" s="63" t="s">
+        <v>281</v>
+      </c>
+      <c r="F26" s="50">
+        <v>631</v>
+      </c>
+      <c r="G26" s="50">
+        <v>631</v>
+      </c>
+      <c r="H26" s="63" t="s">
+        <v>281</v>
+      </c>
+      <c r="I26" s="63" t="s">
+        <v>281</v>
+      </c>
+      <c r="J26" s="63" t="s">
+        <v>281</v>
+      </c>
+      <c r="K26" s="63" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C27" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G27" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="H27" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="I27" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="J27" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="K27" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C28" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="H28" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="I28" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="J28" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="K28" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C29" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G29" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="H29" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="I29" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="J29" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="K29" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C30" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G30" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="H30" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="I30" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="J30" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="K30" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C31" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G31" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="H31" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="I31" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="J31" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="K31" s="35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C32" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="41">
+        <v>-1.4498E-2</v>
+      </c>
+      <c r="E32" s="45">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="F32" s="41">
+        <v>-1.7427999999999999E-2</v>
+      </c>
+      <c r="G32" s="45">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="H32" s="41">
+        <v>-3.7006299999999999E-2</v>
+      </c>
+      <c r="I32" s="45">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="J32" s="45">
+        <v>-3.4202000000000003E-2</v>
+      </c>
+      <c r="K32" s="45">
+        <v>0.11899999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C33" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="41">
+        <v>3.2797999999999998E-3</v>
+      </c>
+      <c r="E33" s="45">
+        <v>0.308</v>
+      </c>
+      <c r="F33" s="41">
+        <v>-6.4300000000000004E-5</v>
+      </c>
+      <c r="G33" s="45">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="H33" s="41">
+        <v>1.7842999999999999E-3</v>
+      </c>
+      <c r="I33" s="45">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="J33" s="45">
+        <v>1.9859000000000001E-3</v>
+      </c>
+      <c r="K33" s="45">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C34" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="41">
+        <v>-1.1218199999999999E-2</v>
+      </c>
+      <c r="E34" s="45">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="F34" s="41">
+        <v>-1.7492299999999999E-2</v>
+      </c>
+      <c r="G34" s="45">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="H34" s="47">
+        <v>-3.5222000000000003E-2</v>
+      </c>
+      <c r="I34" s="47">
+        <v>0.308</v>
+      </c>
+      <c r="J34" s="41">
+        <v>-3.2216099999999998E-2</v>
+      </c>
+      <c r="K34" s="45">
+        <v>0.14099999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C35" s="37"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="38"/>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C36" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C37" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+    </row>
+    <row r="42" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="D42" s="46"/>
+    </row>
+    <row r="43" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C43" s="27" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="44" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="D44" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" s="59"/>
+      <c r="F44" s="59"/>
+      <c r="G44" s="59"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
+      <c r="K44" s="59"/>
+    </row>
+    <row r="45" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="D45" s="56">
+        <v>1</v>
+      </c>
+      <c r="E45" s="56">
+        <v>2</v>
+      </c>
+      <c r="F45" s="28">
+        <v>3</v>
+      </c>
+      <c r="G45" s="28">
+        <v>4</v>
+      </c>
+      <c r="H45" s="56">
+        <v>5</v>
+      </c>
+      <c r="I45" s="56">
+        <v>6</v>
+      </c>
+      <c r="J45" s="56">
+        <v>7</v>
+      </c>
+      <c r="K45" s="56">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="3:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C46" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="D46" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="E46" s="43" t="s">
+        <v>491</v>
+      </c>
+      <c r="F46" s="43" t="s">
+        <v>258</v>
+      </c>
+      <c r="G46" s="43" t="s">
+        <v>491</v>
+      </c>
+      <c r="H46" s="43" t="s">
+        <v>259</v>
+      </c>
+      <c r="I46" s="43" t="s">
+        <v>491</v>
+      </c>
+      <c r="J46" s="43" t="s">
+        <v>260</v>
+      </c>
+      <c r="K46" s="43" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="47" spans="3:11" ht="16" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="C47" s="27" t="s">
+        <v>331</v>
+      </c>
+      <c r="D47" s="44" t="s">
+        <v>506</v>
+      </c>
+      <c r="E47" s="44" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="48" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C48" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="E48" s="44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C49" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="44" t="s">
+        <v>510</v>
+      </c>
+      <c r="G49" s="44" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="50" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C50" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="G50" s="44" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C51" s="27" t="s">
+        <v>333</v>
+      </c>
+      <c r="D51" s="46"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="49"/>
+      <c r="H51" s="44" t="s">
+        <v>437</v>
+      </c>
+      <c r="I51" s="44" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="52" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C52" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="46"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="49"/>
+      <c r="H52" s="44" t="s">
+        <v>363</v>
+      </c>
+      <c r="I52" s="44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C53" s="27" t="s">
+        <v>334</v>
+      </c>
+      <c r="D53" s="46"/>
+      <c r="E53" s="46"/>
+      <c r="H53" s="44"/>
+      <c r="I53" s="44"/>
+      <c r="J53" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="K53" s="44" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="54" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C54" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" s="46"/>
+      <c r="E54" s="46"/>
+      <c r="H54" s="49"/>
+      <c r="I54" s="49"/>
+      <c r="J54" s="44" t="s">
+        <v>245</v>
+      </c>
+      <c r="K54" s="44" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C55" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D55" s="46"/>
+      <c r="E55" s="44" t="s">
+        <v>481</v>
+      </c>
+      <c r="G55" s="44" t="s">
+        <v>484</v>
+      </c>
+      <c r="I55" s="44" t="s">
+        <v>481</v>
+      </c>
+      <c r="K55" s="44" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="56" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C56" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="46"/>
+      <c r="E56" s="44" t="s">
+        <v>493</v>
+      </c>
+      <c r="G56" s="44" t="s">
+        <v>493</v>
+      </c>
+      <c r="I56" s="44" t="s">
+        <v>493</v>
+      </c>
+      <c r="K56" s="44" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="57" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C57" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D57" s="44" t="s">
+        <v>390</v>
+      </c>
+      <c r="E57" s="44" t="s">
+        <v>370</v>
+      </c>
+      <c r="F57" s="44" t="s">
+        <v>402</v>
+      </c>
+      <c r="G57" s="44" t="s">
+        <v>370</v>
+      </c>
+      <c r="H57" s="44" t="s">
+        <v>390</v>
+      </c>
+      <c r="I57" s="44" t="s">
+        <v>370</v>
+      </c>
+      <c r="J57" s="44" t="s">
+        <v>372</v>
+      </c>
+      <c r="K57" s="44" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="58" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C58" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="E58" s="44" t="s">
+        <v>495</v>
+      </c>
+      <c r="F58" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="G58" s="44" t="s">
+        <v>495</v>
+      </c>
+      <c r="H58" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="I58" s="44" t="s">
+        <v>495</v>
+      </c>
+      <c r="J58" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="K58" s="44" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="59" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C59" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="D59" s="44" t="s">
+        <v>272</v>
+      </c>
+      <c r="E59" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="F59" s="44" t="s">
+        <v>425</v>
+      </c>
+      <c r="G59" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="H59" s="44" t="s">
+        <v>365</v>
+      </c>
+      <c r="I59" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="J59" s="44" t="s">
+        <v>365</v>
+      </c>
+      <c r="K59" s="44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="D60" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="E60" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="F60" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="G60" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="H60" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="I60" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="J60" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="K60" s="44" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="61" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C61" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="D61" s="44" t="s">
+        <v>507</v>
+      </c>
+      <c r="E61" s="44" t="s">
+        <v>508</v>
+      </c>
+      <c r="F61" s="44" t="s">
+        <v>338</v>
+      </c>
+      <c r="G61" s="44" t="s">
+        <v>511</v>
+      </c>
+      <c r="H61" s="44" t="s">
+        <v>507</v>
+      </c>
+      <c r="I61" s="44" t="s">
+        <v>512</v>
+      </c>
+      <c r="J61" s="44" t="s">
+        <v>514</v>
+      </c>
+      <c r="K61" s="44" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="62" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="D62" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E62" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="F62" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="G62" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="H62" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="I62" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="J62" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="K62" s="44" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="63" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C63" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D63" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="E63" s="44" t="s">
+        <v>509</v>
+      </c>
+      <c r="F63" s="44" t="s">
+        <v>354</v>
+      </c>
+      <c r="G63" s="44" t="s">
+        <v>370</v>
+      </c>
+      <c r="H63" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="I63" s="44" t="s">
+        <v>513</v>
+      </c>
+      <c r="J63" s="44" t="s">
+        <v>350</v>
+      </c>
+      <c r="K63" s="44" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="64" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C64" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" s="44" t="s">
+        <v>276</v>
+      </c>
+      <c r="E64" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="F64" s="44" t="s">
+        <v>276</v>
+      </c>
+      <c r="G64" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="H64" s="44" t="s">
+        <v>317</v>
+      </c>
+      <c r="I64" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="J64" s="44" t="s">
+        <v>317</v>
+      </c>
+      <c r="K64" s="44" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="65" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C65" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="D65" s="44"/>
+      <c r="E65" s="44"/>
+      <c r="F65" s="44"/>
+      <c r="G65" s="44"/>
+      <c r="H65" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="I65" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="J65" s="44"/>
+      <c r="K65" s="44"/>
+    </row>
+    <row r="66" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C66" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" s="44"/>
+      <c r="E66" s="44"/>
+      <c r="F66" s="44"/>
+      <c r="G66" s="44"/>
+      <c r="H66" s="44"/>
+      <c r="I66" s="44"/>
+      <c r="J66" s="44"/>
+      <c r="K66" s="44"/>
+    </row>
+    <row r="67" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C67" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F67" s="28"/>
+      <c r="G67" s="28"/>
+    </row>
+    <row r="68" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C68" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D68" s="63" t="s">
+        <v>281</v>
+      </c>
+      <c r="E68" s="63" t="s">
+        <v>281</v>
+      </c>
+      <c r="F68" s="63" t="s">
+        <v>281</v>
+      </c>
+      <c r="G68" s="63" t="s">
+        <v>281</v>
+      </c>
+      <c r="H68" s="63" t="s">
+        <v>281</v>
+      </c>
+      <c r="I68" s="63" t="s">
+        <v>281</v>
+      </c>
+      <c r="J68" s="63" t="s">
+        <v>281</v>
+      </c>
+      <c r="K68" s="63" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="69" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C69" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D69" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E69" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F69" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G69" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="H69" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="I69" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="J69" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="K69" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="70" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C70" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D70" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E70" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F70" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G70" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="H70" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="I70" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="J70" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="K70" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="71" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C71" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="D71" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E71" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F71" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G71" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="H71" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="I71" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="J71" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="K71" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="72" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C72" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D72" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E72" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F72" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G72" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="H72" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="I72" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="J72" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="K72" s="31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="73" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C73" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="D73" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="E73" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F73" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G73" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="H73" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="I73" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="J73" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="K73" s="35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="74" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C74" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="D74" s="41">
+        <v>-3.3355999999999997E-2</v>
+      </c>
+      <c r="E74" s="45">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="F74" s="41">
+        <v>-2.9586999999999999E-2</v>
+      </c>
+      <c r="G74" s="45">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="H74" s="41">
+        <v>-4.06708E-2</v>
+      </c>
+      <c r="I74" s="45">
+        <v>0.104</v>
+      </c>
+      <c r="J74" s="45">
+        <v>-2.98461E-2</v>
+      </c>
+      <c r="K74" s="45">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C75" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="D75" s="41">
+        <v>1.2727000000000001E-3</v>
+      </c>
+      <c r="E75" s="45">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="F75" s="41">
+        <v>1.6257999999999999E-3</v>
+      </c>
+      <c r="G75" s="45">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="H75" s="41">
+        <v>6.8199999999999999E-4</v>
+      </c>
+      <c r="I75" s="45">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="J75" s="45">
+        <v>6.0300000000000002E-5</v>
+      </c>
+      <c r="K75" s="45">
+        <v>0.94499999999999995</v>
+      </c>
+    </row>
+    <row r="76" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C76" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="D76" s="41">
+        <v>-3.2083300000000002E-2</v>
+      </c>
+      <c r="E76" s="45">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="F76" s="41">
+        <v>-2.7962000000000001E-2</v>
+      </c>
+      <c r="G76" s="45">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="H76" s="47">
+        <v>-3.9988000000000003E-2</v>
+      </c>
+      <c r="I76" s="47">
+        <v>0.11</v>
+      </c>
+      <c r="J76" s="41">
+        <v>-2.9785800000000001E-2</v>
+      </c>
+      <c r="K76" s="41">
+        <v>0.14099999999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C77" s="37"/>
+      <c r="D77" s="38"/>
+      <c r="E77" s="38"/>
+      <c r="F77" s="38"/>
+      <c r="G77" s="38"/>
+      <c r="H77" s="38"/>
+      <c r="I77" s="38"/>
+      <c r="J77" s="38"/>
+      <c r="K77" s="38"/>
+    </row>
+    <row r="78" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C78" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="D78" s="40"/>
+      <c r="E78" s="40"/>
+    </row>
+    <row r="79" spans="3:11" x14ac:dyDescent="0.35">
+      <c r="C79" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D79" s="40"/>
+      <c r="E79" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D2:K2"/>
+    <mergeCell ref="D44:K44"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K44"/>
   <sheetViews>
@@ -7065,16 +8715,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.35">
       <c r="D3" s="42">
@@ -7135,7 +8785,7 @@
       <c r="C5" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="58" t="s">
         <v>124</v>
       </c>
       <c r="E5" s="44" t="s">
@@ -7146,7 +8796,7 @@
       <c r="C6" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="62" t="s">
+      <c r="D6" s="58" t="s">
         <v>126</v>
       </c>
       <c r="E6" s="44" t="s">
@@ -7159,7 +8809,7 @@
       </c>
       <c r="D7" s="46"/>
       <c r="E7" s="46"/>
-      <c r="F7" s="62" t="s">
+      <c r="F7" s="58" t="s">
         <v>150</v>
       </c>
       <c r="G7" s="44" t="s">
@@ -7172,7 +8822,7 @@
       </c>
       <c r="D8" s="46"/>
       <c r="E8" s="46"/>
-      <c r="F8" s="62" t="s">
+      <c r="F8" s="58" t="s">
         <v>152</v>
       </c>
       <c r="G8" s="44" t="s">
@@ -7185,8 +8835,8 @@
       </c>
       <c r="D9" s="46"/>
       <c r="E9" s="46"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
     </row>
     <row r="10" spans="3:11" x14ac:dyDescent="0.35">
       <c r="C10" s="27" t="s">
@@ -7194,9 +8844,9 @@
       </c>
       <c r="D10" s="46"/>
       <c r="E10" s="46"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="62" t="s">
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="58" t="s">
         <v>177</v>
       </c>
       <c r="I10" s="44" t="s">
@@ -7209,13 +8859,13 @@
       </c>
       <c r="D11" s="46"/>
       <c r="E11" s="46"/>
-      <c r="H11" s="62" t="s">
+      <c r="H11" s="58" t="s">
         <v>111</v>
       </c>
       <c r="I11" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="J11" s="62" t="s">
+      <c r="J11" s="58" t="s">
         <v>194</v>
       </c>
       <c r="K11" s="44" t="s">
@@ -7228,9 +8878,9 @@
       </c>
       <c r="D12" s="46"/>
       <c r="E12" s="46"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="62" t="s">
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="58" t="s">
         <v>41</v>
       </c>
       <c r="K12" s="44" t="s">
@@ -7238,20 +8888,20 @@
       </c>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="48" t="s">
         <v>100</v>
       </c>
       <c r="D13" s="46"/>
-      <c r="E13" s="62" t="s">
+      <c r="E13" s="58" t="s">
         <v>128</v>
       </c>
-      <c r="G13" s="62" t="s">
+      <c r="G13" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="I13" s="62" t="s">
+      <c r="I13" s="58" t="s">
         <v>175</v>
       </c>
-      <c r="K13" s="62" t="s">
+      <c r="K13" s="58" t="s">
         <v>192</v>
       </c>
     </row>
@@ -7260,16 +8910,16 @@
         <v>4</v>
       </c>
       <c r="D14" s="46"/>
-      <c r="E14" s="62" t="s">
+      <c r="E14" s="58" t="s">
         <v>129</v>
       </c>
-      <c r="G14" s="62" t="s">
+      <c r="G14" s="58" t="s">
         <v>155</v>
       </c>
-      <c r="I14" s="62" t="s">
+      <c r="I14" s="58" t="s">
         <v>176</v>
       </c>
-      <c r="K14" s="62" t="s">
+      <c r="K14" s="58" t="s">
         <v>193</v>
       </c>
     </row>
@@ -7555,7 +9205,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C25" s="51" t="s">
+      <c r="C25" s="48" t="s">
         <v>101</v>
       </c>
       <c r="D25" s="44" t="s">
@@ -7623,28 +9273,28 @@
       <c r="C28" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="54" t="s">
+      <c r="D28" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="E28" s="54" t="s">
+      <c r="E28" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="F28" s="54" t="s">
+      <c r="F28" s="50" t="s">
         <v>174</v>
       </c>
-      <c r="G28" s="54" t="s">
+      <c r="G28" s="50" t="s">
         <v>174</v>
       </c>
-      <c r="H28" s="54" t="s">
+      <c r="H28" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="I28" s="54" t="s">
+      <c r="I28" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="J28" s="54" t="s">
+      <c r="J28" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="K28" s="54" t="s">
+      <c r="K28" s="50" t="s">
         <v>123</v>
       </c>
     </row>
@@ -7710,31 +9360,31 @@
       <c r="A31" s="27" t="s">
         <v>208</v>
       </c>
-      <c r="C31" s="57" t="s">
+      <c r="C31" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="59" t="s">
+      <c r="D31" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="E31" s="59" t="s">
+      <c r="E31" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="F31" s="59" t="s">
+      <c r="F31" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="G31" s="59" t="s">
+      <c r="G31" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="H31" s="59" t="s">
+      <c r="H31" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="I31" s="59" t="s">
+      <c r="I31" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="J31" s="59" t="s">
+      <c r="J31" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="K31" s="59" t="s">
+      <c r="K31" s="55" t="s">
         <v>122</v>
       </c>
     </row>
@@ -7832,7 +9482,7 @@
       <c r="D35" s="41">
         <v>9.3230400000000005E-2</v>
       </c>
-      <c r="E35" s="56">
+      <c r="E35" s="52">
         <v>6.3E-2</v>
       </c>
       <c r="F35" s="41">
@@ -7850,7 +9500,7 @@
       <c r="J35" s="41">
         <v>7.1631700000000006E-2</v>
       </c>
-      <c r="K35" s="55">
+      <c r="K35" s="51">
         <v>9.7000000000000003E-2</v>
       </c>
     </row>
@@ -7909,7 +9559,7 @@
       <c r="E39" s="40"/>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="D44" s="58" t="s">
+      <c r="D44" s="54" t="s">
         <v>121</v>
       </c>
     </row>
@@ -7922,7 +9572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K44"/>
   <sheetViews>
@@ -7946,16 +9596,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
     </row>
     <row r="3" spans="3:11" x14ac:dyDescent="0.35">
       <c r="D3" s="42">
@@ -8016,7 +9666,7 @@
       <c r="C5" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="58" t="s">
         <v>228</v>
       </c>
       <c r="E5" s="44" t="s">
@@ -8027,7 +9677,7 @@
       <c r="C6" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="62" t="s">
+      <c r="D6" s="58" t="s">
         <v>126</v>
       </c>
       <c r="E6" s="44" t="s">
@@ -8066,9 +9716,9 @@
       </c>
       <c r="D9" s="46"/>
       <c r="E9" s="46"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="62" t="s">
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="58" t="s">
         <v>209</v>
       </c>
       <c r="I9" s="44" t="s">
@@ -8081,9 +9731,9 @@
       </c>
       <c r="D10" s="46"/>
       <c r="E10" s="46"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="62" t="s">
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="58" t="s">
         <v>111</v>
       </c>
       <c r="I10" s="44" t="s">
@@ -8098,7 +9748,7 @@
       <c r="E11" s="46"/>
       <c r="H11" s="44"/>
       <c r="I11" s="44"/>
-      <c r="J11" s="62" t="s">
+      <c r="J11" s="58" t="s">
         <v>228</v>
       </c>
       <c r="K11" s="44" t="s">
@@ -8111,9 +9761,9 @@
       </c>
       <c r="D12" s="46"/>
       <c r="E12" s="46"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="62" t="s">
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="58" t="s">
         <v>126</v>
       </c>
       <c r="K12" s="44" t="s">
@@ -8121,20 +9771,20 @@
       </c>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="48" t="s">
         <v>100</v>
       </c>
       <c r="D13" s="46"/>
-      <c r="E13" s="62" t="s">
+      <c r="E13" s="58" t="s">
         <v>231</v>
       </c>
       <c r="G13" s="44" t="s">
         <v>242</v>
       </c>
-      <c r="I13" s="62" t="s">
+      <c r="I13" s="58" t="s">
         <v>212</v>
       </c>
-      <c r="K13" s="62" t="s">
+      <c r="K13" s="58" t="s">
         <v>231</v>
       </c>
     </row>
@@ -8143,16 +9793,16 @@
         <v>4</v>
       </c>
       <c r="D14" s="46"/>
-      <c r="E14" s="62" t="s">
+      <c r="E14" s="58" t="s">
         <v>232</v>
       </c>
       <c r="G14" s="44" t="s">
         <v>243</v>
       </c>
-      <c r="I14" s="62" t="s">
+      <c r="I14" s="58" t="s">
         <v>213</v>
       </c>
-      <c r="K14" s="62" t="s">
+      <c r="K14" s="58" t="s">
         <v>232</v>
       </c>
     </row>
@@ -8438,7 +10088,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C25" s="51" t="s">
+      <c r="C25" s="48" t="s">
         <v>101</v>
       </c>
       <c r="D25" s="44" t="s">
@@ -8506,24 +10156,24 @@
       <c r="C28" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="54" t="s">
+      <c r="D28" s="50" t="s">
         <v>227</v>
       </c>
-      <c r="E28" s="54" t="s">
+      <c r="E28" s="50" t="s">
         <v>227</v>
       </c>
-      <c r="F28" s="54"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="54" t="s">
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50" t="s">
         <v>227</v>
       </c>
-      <c r="I28" s="54" t="s">
+      <c r="I28" s="50" t="s">
         <v>227</v>
       </c>
-      <c r="J28" s="54" t="s">
+      <c r="J28" s="50" t="s">
         <v>227</v>
       </c>
-      <c r="K28" s="54" t="s">
+      <c r="K28" s="50" t="s">
         <v>227</v>
       </c>
     </row>
@@ -8589,31 +10239,31 @@
       <c r="A31" s="27" t="s">
         <v>208</v>
       </c>
-      <c r="C31" s="57" t="s">
+      <c r="C31" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="59" t="s">
+      <c r="D31" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="E31" s="59" t="s">
+      <c r="E31" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="F31" s="59" t="s">
+      <c r="F31" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="G31" s="59" t="s">
+      <c r="G31" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="H31" s="59" t="s">
+      <c r="H31" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="I31" s="59" t="s">
+      <c r="I31" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="J31" s="59" t="s">
+      <c r="J31" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="K31" s="59" t="s">
+      <c r="K31" s="55" t="s">
         <v>122</v>
       </c>
     </row>
@@ -8711,7 +10361,7 @@
       <c r="D35" s="41">
         <v>-8.6108500000000004E-2</v>
       </c>
-      <c r="E35" s="55">
+      <c r="E35" s="51">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="F35" s="41">
@@ -8723,13 +10373,13 @@
       <c r="H35" s="41">
         <v>-5.7638799999999997E-2</v>
       </c>
-      <c r="I35" s="55">
+      <c r="I35" s="51">
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="J35" s="41">
         <v>-8.6108500000000004E-2</v>
       </c>
-      <c r="K35" s="55">
+      <c r="K35" s="51">
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
@@ -8788,7 +10438,7 @@
       <c r="E39" s="40"/>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.35">
-      <c r="D44" s="58" t="s">
+      <c r="D44" s="54" t="s">
         <v>121</v>
       </c>
     </row>
@@ -8800,7 +10450,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:I42"/>
   <sheetViews>
@@ -8815,14 +10465,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.35">
       <c r="D4" s="1"/>
@@ -8878,7 +10528,7 @@
       <c r="H7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="49" t="s">
+      <c r="I7" s="61" t="s">
         <v>77</v>
       </c>
     </row>
@@ -8901,7 +10551,7 @@
       <c r="H8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="49"/>
+      <c r="I8" s="61"/>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.35">
       <c r="D9" s="3" t="s">
@@ -8919,7 +10569,7 @@
       <c r="H9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I9" s="49"/>
+      <c r="I9" s="61"/>
     </row>
     <row r="10" spans="3:9" ht="28" x14ac:dyDescent="0.35">
       <c r="C10" s="25" t="s">
@@ -8940,7 +10590,7 @@
       <c r="H10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="49"/>
+      <c r="I10" s="61"/>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.35">
       <c r="D11" s="3" t="s">
@@ -8958,7 +10608,7 @@
       <c r="H11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="49"/>
+      <c r="I11" s="61"/>
     </row>
     <row r="12" spans="3:9" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D12" s="22" t="s">
@@ -8976,7 +10626,7 @@
       <c r="H12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="49"/>
+      <c r="I12" s="61"/>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C13" s="26"/>
@@ -8995,10 +10645,10 @@
       <c r="H13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="49"/>
+      <c r="I13" s="61"/>
     </row>
     <row r="14" spans="3:9" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="60" t="s">
         <v>83</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -9016,10 +10666,10 @@
       <c r="H14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I14" s="49"/>
+      <c r="I14" s="61"/>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C15" s="48"/>
+      <c r="C15" s="60"/>
       <c r="D15" s="3" t="s">
         <v>4</v>
       </c>
@@ -9035,10 +10685,10 @@
       <c r="H15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="49"/>
+      <c r="I15" s="61"/>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C16" s="48"/>
+      <c r="C16" s="60"/>
       <c r="D16" s="3" t="s">
         <v>28</v>
       </c>
@@ -9054,10 +10704,10 @@
       <c r="H16" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I16" s="49"/>
+      <c r="I16" s="61"/>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C17" s="48"/>
+      <c r="C17" s="60"/>
       <c r="D17" s="3" t="s">
         <v>4</v>
       </c>
@@ -9073,10 +10723,10 @@
       <c r="H17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="49"/>
+      <c r="I17" s="61"/>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C18" s="48"/>
+      <c r="C18" s="60"/>
       <c r="D18" s="3" t="s">
         <v>32</v>
       </c>
@@ -9092,7 +10742,7 @@
       <c r="H18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I18" s="49"/>
+      <c r="I18" s="61"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C19" s="1"/>
@@ -9111,7 +10761,7 @@
       <c r="H19" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="I19" s="49"/>
+      <c r="I19" s="61"/>
     </row>
     <row r="20" spans="3:9" ht="28" x14ac:dyDescent="0.35">
       <c r="C20" s="25" t="s">
@@ -9132,7 +10782,7 @@
       <c r="H20" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I20" s="49"/>
+      <c r="I20" s="61"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C21" s="1"/>
@@ -9151,10 +10801,10 @@
       <c r="H21" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="I21" s="49"/>
+      <c r="I21" s="61"/>
     </row>
     <row r="22" spans="3:9" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="48" t="s">
+      <c r="C22" s="60" t="s">
         <v>83</v>
       </c>
       <c r="D22" s="3" t="s">
@@ -9172,10 +10822,10 @@
       <c r="H22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I22" s="49"/>
+      <c r="I22" s="61"/>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C23" s="48"/>
+      <c r="C23" s="60"/>
       <c r="D23" s="3" t="s">
         <v>4</v>
       </c>
@@ -9191,10 +10841,10 @@
       <c r="H23" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I23" s="49"/>
+      <c r="I23" s="61"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C24" s="48"/>
+      <c r="C24" s="60"/>
       <c r="D24" s="3" t="s">
         <v>46</v>
       </c>
@@ -9210,10 +10860,10 @@
       <c r="H24" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I24" s="49"/>
+      <c r="I24" s="61"/>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C25" s="48"/>
+      <c r="C25" s="60"/>
       <c r="D25" s="3"/>
       <c r="E25" s="6" t="s">
         <v>49</v>
@@ -9227,10 +10877,10 @@
       <c r="H25" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I25" s="49"/>
+      <c r="I25" s="61"/>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C26" s="48"/>
+      <c r="C26" s="60"/>
       <c r="D26" s="3" t="s">
         <v>50</v>
       </c>
@@ -9246,7 +10896,7 @@
       <c r="H26" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="I26" s="49"/>
+      <c r="I26" s="61"/>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C27" s="23"/>
@@ -9263,7 +10913,7 @@
       <c r="H27" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="I27" s="49"/>
+      <c r="I27" s="61"/>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C28" s="23"/>
@@ -9272,7 +10922,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="49"/>
+      <c r="I28" s="61"/>
     </row>
     <row r="29" spans="3:9" x14ac:dyDescent="0.35">
       <c r="D29" s="16" t="s">
@@ -9290,7 +10940,7 @@
       <c r="H29" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="I29" s="49"/>
+      <c r="I29" s="61"/>
     </row>
     <row r="30" spans="3:9" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D30" s="18" t="s">
@@ -9308,7 +10958,7 @@
       <c r="H30" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="I30" s="49"/>
+      <c r="I30" s="61"/>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.35">
       <c r="D31" s="20" t="s">
@@ -9326,7 +10976,7 @@
       <c r="H31" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="I31" s="49"/>
+      <c r="I31" s="61"/>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.35">
       <c r="D32" s="21" t="s">
@@ -9344,7 +10994,7 @@
       <c r="H32" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="I32" s="49"/>
+      <c r="I32" s="61"/>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D33" s="21" t="s">
@@ -9362,7 +11012,7 @@
       <c r="H33" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="I33" s="49"/>
+      <c r="I33" s="61"/>
     </row>
     <row r="34" spans="4:9" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D34" s="8"/>
@@ -9370,7 +11020,7 @@
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
-      <c r="I34" s="49" t="s">
+      <c r="I34" s="61" t="s">
         <v>76</v>
       </c>
     </row>
@@ -9390,7 +11040,7 @@
       <c r="H35" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="I35" s="49"/>
+      <c r="I35" s="61"/>
     </row>
     <row r="36" spans="4:9" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D36" s="12" t="s">
@@ -9408,7 +11058,7 @@
       <c r="H36" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="I36" s="49"/>
+      <c r="I36" s="61"/>
     </row>
     <row r="37" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D37" s="12" t="s">
@@ -9426,7 +11076,7 @@
       <c r="H37" s="13">
         <v>0.124</v>
       </c>
-      <c r="I37" s="49"/>
+      <c r="I37" s="61"/>
     </row>
     <row r="38" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D38" s="12" t="s">
@@ -9444,7 +11094,7 @@
       <c r="H38" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="I38" s="49"/>
+      <c r="I38" s="61"/>
     </row>
     <row r="39" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D39" s="14"/>
@@ -9460,7 +11110,7 @@
       <c r="H39" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I39" s="49"/>
+      <c r="I39" s="61"/>
     </row>
     <row r="40" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D40" s="15" t="s">

</xml_diff>